<commit_message>
update guru, siswa jurnal
</commit_message>
<xml_diff>
--- a/public/excel/siswa -1.xlsx
+++ b/public/excel/siswa -1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MY\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C08B9E5-7227-46AF-B3C5-9AA3088A1684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DA8B67-EA1B-4205-8C2D-B18176AD8483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F295664A-43F9-4F05-B0EE-BC8DB2B9BFE9}"/>
   </bookViews>
@@ -25,30 +25,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>nis</t>
   </si>
   <si>
+    <t>nm_siswa</t>
+  </si>
+  <si>
+    <t>tmpt_lhr</t>
+  </si>
+  <si>
+    <t>tgl_lhr</t>
+  </si>
+  <si>
+    <t>jen_kel</t>
+  </si>
+  <si>
+    <t>agama</t>
+  </si>
+  <si>
+    <t>almt_siswa</t>
+  </si>
+  <si>
+    <t>no_tlp</t>
+  </si>
+  <si>
     <t>nisn</t>
   </si>
   <si>
+    <t>nm_ayah</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>kelas_id</t>
   </si>
   <si>
     <t>Ket: kelas_id lihat di master-&gt;kelas</t>
   </si>
   <si>
-    <t>Ket: tp_id lihat di master-&gt;TP</t>
-  </si>
-  <si>
     <t>xxxx</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>nama</t>
+    <t>2004-02-10</t>
+  </si>
+  <si>
+    <t>Ket: tgl_lahir pengisian= thn-bln-tgl, contoh: '2021-01-15</t>
   </si>
 </sst>
 </file>
@@ -473,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2ED6C48-B5A4-4972-B7FF-1DDB3FF99FC4}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,49 +508,89 @@
     <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>80010</v>
       </c>
-      <c r="B2" s="5">
-        <v>12222</v>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>3</v>
+      <c r="L2" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F3" s="6" t="s">
-        <v>4</v>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>